<commit_message>
v0.3.0 - Consistency in teacher assignments
</commit_message>
<xml_diff>
--- a/Outputs/excel/visual_timetable.xlsx
+++ b/Outputs/excel/visual_timetable.xlsx
@@ -12,23 +12,24 @@
     <sheet name="Group_A1_TDA_W1" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Group_A2_TDA_W2" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Group_A2_TDA_W1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Teacher_Barbeau_Henri_W2" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Teacher_Barbeau_Henri_W1" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Teacher_Solé_Timothé_W1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Teacher_Cerfbeer_Renaud_W1" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Teacher_Cerfbeer_Renaud_W2" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Teacher_Poussin_Constantin_W1" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Teacher_Poussin_Constantin_W2" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Teacher_Brunelle_Christiane_W1" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Teacher_Brunelle_Christiane_W2" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Teacher_Vannier_Maurice_W1" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Teacher_Vannier_Maurice_W2" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Room_L101_W2" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Room_L101_W1" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Room_L103_W1" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="Room_L103_W2" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Teacher_Solé_Timothé_W2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Teacher_Solé_Timothé_W1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Teacher_Poussin_Constantin_W1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Teacher_Poussin_Constantin_W2" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Teacher_Brunelle_Christiane_W1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Teacher_Brunelle_Christiane_W2" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Teacher_Barbeau_Henri_W2" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Teacher_Barbeau_Henri_W1" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Teacher_Cerfbeer_Renaud_W1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Teacher_Cerfbeer_Renaud_W2" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Teacher_Vannier_Maurice_W1" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Teacher_Vannier_Maurice_W2" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Room_L101_W2" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Room_L101_W1" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Room_L102_W2" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="Room_L102_W1" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="Room_L102_W2" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Room_Online_W1" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Room_L103_W2" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -38,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -63,6 +64,9 @@
     </font>
     <font>
       <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <sz val="8"/>
     </font>
     <font>
       <b val="1"/>
@@ -189,30 +193,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -227,23 +231,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -611,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -838,7 +845,7 @@
       </c>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>Week 1</t>
+          <t>Week 2</t>
         </is>
       </c>
     </row>
@@ -855,12 +862,12 @@
       </c>
       <c r="G9" s="6" t="inlineStr">
         <is>
-          <t>L103</t>
+          <t>Online</t>
         </is>
       </c>
       <c r="H9" s="7" t="inlineStr">
         <is>
-          <t>Week 2</t>
+          <t>Week 1</t>
         </is>
       </c>
     </row>
@@ -903,12 +910,12 @@
     <row r="13">
       <c r="D13" s="6" t="inlineStr">
         <is>
-          <t>Vannier_Maurice</t>
+          <t>Solé_Timothé</t>
         </is>
       </c>
       <c r="E13" s="7" t="inlineStr">
         <is>
-          <t>Week 1</t>
+          <t>Week 2</t>
         </is>
       </c>
     </row>
@@ -920,28 +927,40 @@
       </c>
       <c r="E14" s="7" t="inlineStr">
         <is>
+          <t>Week 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="6" t="inlineStr">
+        <is>
+          <t>Vannier_Maurice</t>
+        </is>
+      </c>
+      <c r="E15" s="7" t="inlineStr">
+        <is>
           <t>Week 2</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="8" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="8" t="inlineStr">
         <is>
           <t>Click on any name to view the corresponding timetable</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="8" t="inlineStr">
-        <is>
-          <t>ESILV - Generated on 26/02/2025 15:44</t>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>ESILV - Generated on 26/02/2025 15:59</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:H20"/>
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
@@ -966,6 +985,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D12" r:id="rId19"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D13" r:id="rId20"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D14" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D15" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -998,7 +1018,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Cerfbeer_Renaud - Week 2: 13/01/2025 - 19/01/2025</t>
+          <t>Teacher: Brunelle_Christiane - Week 1: 06/01/2025 - 12/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -1056,23 +1076,17 @@
         </is>
       </c>
       <c r="B3" s="14" t="n"/>
-      <c r="C3" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
-      <c r="D3" s="14" t="n"/>
+      <c r="C3" s="14" t="n"/>
+      <c r="D3" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L102)</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="n"/>
       <c r="F3" s="14" t="n"/>
-      <c r="G3" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
+      <c r="G3" s="14" t="n"/>
       <c r="H3" s="14" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
@@ -1081,24 +1095,24 @@
           <t>10:00 - 11:30</t>
         </is>
       </c>
-      <c r="B4" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
+      <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n"/>
       <c r="D4" s="16" t="inlineStr">
         <is>
-          <t>Basic Physics
-Renaud Cerfbeer
+          <t>Basic Informatics
+Christiane Brunelle
 (L102)</t>
         </is>
       </c>
       <c r="E4" s="14" t="n"/>
       <c r="F4" s="14" t="n"/>
-      <c r="G4" s="14" t="n"/>
+      <c r="G4" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(Online)</t>
+        </is>
+      </c>
       <c r="H4" s="14" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
@@ -1121,21 +1135,9 @@
           <t>13:30 - 15:00</t>
         </is>
       </c>
-      <c r="B6" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
+      <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
-      <c r="D6" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n"/>
       <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
@@ -1150,7 +1152,13 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="14" t="n"/>
       <c r="D7" s="14" t="n"/>
-      <c r="E7" s="14" t="n"/>
+      <c r="E7" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L102)</t>
+        </is>
+      </c>
       <c r="F7" s="14" t="n"/>
       <c r="G7" s="14" t="n"/>
       <c r="H7" s="14" t="n"/>
@@ -1161,13 +1169,7 @@
           <t>17:00 - 18:30</t>
         </is>
       </c>
-      <c r="B8" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
       <c r="E8" s="14" t="n"/>
@@ -1181,13 +1183,7 @@
           <t>18:45 - 20:15</t>
         </is>
       </c>
-      <c r="B9" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
+      <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
       <c r="E9" s="14" t="n"/>
@@ -1233,7 +1229,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Poussin_Constantin - Week 1: 06/01/2025 - 12/01/2025</t>
+          <t>Teacher: Brunelle_Christiane - Week 2: 13/01/2025 - 19/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -1294,8 +1290,20 @@
       <c r="C3" s="14" t="n"/>
       <c r="D3" s="14" t="n"/>
       <c r="E3" s="14" t="n"/>
-      <c r="F3" s="14" t="n"/>
-      <c r="G3" s="14" t="n"/>
+      <c r="F3" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L103)</t>
+        </is>
+      </c>
+      <c r="G3" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L101)</t>
+        </is>
+      </c>
       <c r="H3" s="14" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
@@ -1308,7 +1316,13 @@
       <c r="C4" s="14" t="n"/>
       <c r="D4" s="14" t="n"/>
       <c r="E4" s="14" t="n"/>
-      <c r="F4" s="14" t="n"/>
+      <c r="F4" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L101)</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
@@ -1336,7 +1350,13 @@
       <c r="C6" s="14" t="n"/>
       <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n"/>
-      <c r="F6" s="14" t="n"/>
+      <c r="F6" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L102)</t>
+        </is>
+      </c>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
     </row>
@@ -1349,13 +1369,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="14" t="n"/>
       <c r="D7" s="14" t="n"/>
-      <c r="E7" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Constantin Poussin
-(L102)</t>
-        </is>
-      </c>
+      <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n"/>
       <c r="G7" s="14" t="n"/>
       <c r="H7" s="14" t="n"/>
@@ -1366,22 +1380,10 @@
           <t>17:00 - 18:30</t>
         </is>
       </c>
-      <c r="B8" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Constantin Poussin
-(L103)</t>
-        </is>
-      </c>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Constantin Poussin
-(L102)</t>
-        </is>
-      </c>
+      <c r="E8" s="14" t="n"/>
       <c r="F8" s="14" t="n"/>
       <c r="G8" s="14" t="n"/>
       <c r="H8" s="14" t="n"/>
@@ -1395,13 +1397,7 @@
       <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
-      <c r="E9" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Constantin Poussin
-(L103)</t>
-        </is>
-      </c>
+      <c r="E9" s="14" t="n"/>
       <c r="F9" s="14" t="n"/>
       <c r="G9" s="14" t="n"/>
       <c r="H9" s="14" t="n"/>
@@ -1444,7 +1440,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Poussin_Constantin - Week 2: 13/01/2025 - 19/01/2025</t>
+          <t>Teacher: Barbeau_Henri - Week 2: 13/01/2025 - 19/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -1502,17 +1498,23 @@
         </is>
       </c>
       <c r="B3" s="14" t="n"/>
-      <c r="C3" s="14" t="n"/>
-      <c r="D3" s="14" t="n"/>
+      <c r="C3" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
+      <c r="D3" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
       <c r="E3" s="14" t="n"/>
       <c r="F3" s="14" t="n"/>
-      <c r="G3" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Constantin Poussin
-(L101)</t>
-        </is>
-      </c>
+      <c r="G3" s="14" t="n"/>
       <c r="H3" s="14" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
@@ -1521,13 +1523,19 @@
           <t>10:00 - 11:30</t>
         </is>
       </c>
-      <c r="B4" s="14" t="n"/>
+      <c r="B4" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
       <c r="C4" s="14" t="n"/>
       <c r="D4" s="17" t="inlineStr">
         <is>
-          <t>Advanced Physics
-Constantin Poussin
-(L103)</t>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
         </is>
       </c>
       <c r="E4" s="14" t="n"/>
@@ -1643,7 +1651,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Brunelle_Christiane - Week 1: 06/01/2025 - 12/01/2025</t>
+          <t>Teacher: Barbeau_Henri - Week 1: 06/01/2025 - 12/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -1701,17 +1709,17 @@
         </is>
       </c>
       <c r="B3" s="14" t="n"/>
-      <c r="C3" s="14" t="n"/>
+      <c r="C3" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="n"/>
       <c r="E3" s="14" t="n"/>
       <c r="F3" s="14" t="n"/>
-      <c r="G3" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L103)</t>
-        </is>
-      </c>
+      <c r="G3" s="14" t="n"/>
       <c r="H3" s="14" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
@@ -1721,9 +1729,21 @@
         </is>
       </c>
       <c r="B4" s="14" t="n"/>
-      <c r="C4" s="14" t="n"/>
+      <c r="C4" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
       <c r="D4" s="14" t="n"/>
-      <c r="E4" s="14" t="n"/>
+      <c r="E4" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L101)</t>
+        </is>
+      </c>
       <c r="F4" s="14" t="n"/>
       <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
@@ -1748,35 +1768,17 @@
           <t>13:30 - 15:00</t>
         </is>
       </c>
-      <c r="B6" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
+      <c r="B6" s="14" t="n"/>
+      <c r="C6" s="14" t="n"/>
+      <c r="D6" s="14" t="n"/>
+      <c r="E6" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
 (L101)</t>
         </is>
       </c>
-      <c r="C6" s="14" t="n"/>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
-      <c r="E6" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L102)</t>
-        </is>
-      </c>
-      <c r="F6" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
+      <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
     </row>
@@ -1790,13 +1792,7 @@
       <c r="C7" s="14" t="n"/>
       <c r="D7" s="14" t="n"/>
       <c r="E7" s="14" t="n"/>
-      <c r="F7" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
+      <c r="F7" s="14" t="n"/>
       <c r="G7" s="14" t="n"/>
       <c r="H7" s="14" t="n"/>
     </row>
@@ -1866,7 +1862,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Brunelle_Christiane - Week 2: 13/01/2025 - 19/01/2025</t>
+          <t>Teacher: Cerfbeer_Renaud - Week 1: 06/01/2025 - 12/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -1926,21 +1922,15 @@
       <c r="B3" s="14" t="n"/>
       <c r="C3" s="14" t="n"/>
       <c r="D3" s="14" t="n"/>
-      <c r="E3" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
-(L103)</t>
-        </is>
-      </c>
-      <c r="F3" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L103)</t>
-        </is>
-      </c>
-      <c r="G3" s="14" t="n"/>
+      <c r="E3" s="14" t="n"/>
+      <c r="F3" s="14" t="n"/>
+      <c r="G3" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="H3" s="14" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
@@ -1952,17 +1942,11 @@
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n"/>
       <c r="D4" s="14" t="n"/>
-      <c r="E4" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
-      <c r="F4" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
+      <c r="E4" s="14" t="n"/>
+      <c r="F4" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
 (L102)</t>
         </is>
       </c>
@@ -1991,15 +1975,21 @@
       </c>
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
-      <c r="D6" s="14" t="n"/>
-      <c r="E6" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L102)</t>
-        </is>
-      </c>
-      <c r="F6" s="14" t="n"/>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L101)</t>
+        </is>
+      </c>
+      <c r="E6" s="14" t="n"/>
+      <c r="F6" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
     </row>
@@ -2024,13 +2014,7 @@
         </is>
       </c>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
       <c r="E8" s="14" t="n"/>
       <c r="F8" s="14" t="n"/>
@@ -2043,16 +2027,16 @@
           <t>18:45 - 20:15</t>
         </is>
       </c>
-      <c r="B9" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
+      <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
-      <c r="E9" s="14" t="n"/>
+      <c r="E9" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="F9" s="14" t="n"/>
       <c r="G9" s="14" t="n"/>
       <c r="H9" s="14" t="n"/>
@@ -2095,7 +2079,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Vannier_Maurice - Week 1: 06/01/2025 - 12/01/2025</t>
+          <t>Teacher: Cerfbeer_Renaud - Week 2: 13/01/2025 - 19/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -2155,7 +2139,13 @@
       <c r="B3" s="14" t="n"/>
       <c r="C3" s="14" t="n"/>
       <c r="D3" s="14" t="n"/>
-      <c r="E3" s="14" t="n"/>
+      <c r="E3" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="F3" s="14" t="n"/>
       <c r="G3" s="14" t="n"/>
       <c r="H3" s="14" t="n"/>
@@ -2169,7 +2159,13 @@
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n"/>
       <c r="D4" s="14" t="n"/>
-      <c r="E4" s="14" t="n"/>
+      <c r="E4" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="F4" s="14" t="n"/>
       <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
@@ -2197,7 +2193,13 @@
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
       <c r="D6" s="14" t="n"/>
-      <c r="E6" s="14" t="n"/>
+      <c r="E6" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
@@ -2225,14 +2227,14 @@
       <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
-      <c r="E8" s="14" t="n"/>
-      <c r="F8" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Maurice Vannier
-(L102)</t>
-        </is>
-      </c>
+      <c r="E8" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
+      <c r="F8" s="14" t="n"/>
       <c r="G8" s="14" t="n"/>
       <c r="H8" s="14" t="n"/>
     </row>
@@ -2242,16 +2244,16 @@
           <t>18:45 - 20:15</t>
         </is>
       </c>
-      <c r="B9" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Maurice Vannier
-(L101)</t>
-        </is>
-      </c>
+      <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
-      <c r="E9" s="14" t="n"/>
+      <c r="E9" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="F9" s="14" t="n"/>
       <c r="G9" s="14" t="n"/>
       <c r="H9" s="14" t="n"/>
@@ -2294,7 +2296,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Vannier_Maurice - Week 2: 13/01/2025 - 19/01/2025</t>
+          <t>Teacher: Vannier_Maurice - Week 1: 06/01/2025 - 12/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -2351,7 +2353,13 @@
           <t>08:15 - 09:45</t>
         </is>
       </c>
-      <c r="B3" s="14" t="n"/>
+      <c r="B3" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
       <c r="C3" s="14" t="n"/>
       <c r="D3" s="14" t="n"/>
       <c r="E3" s="14" t="n"/>
@@ -2370,7 +2378,13 @@
       <c r="D4" s="14" t="n"/>
       <c r="E4" s="14" t="n"/>
       <c r="F4" s="14" t="n"/>
-      <c r="G4" s="14" t="n"/>
+      <c r="G4" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L101)</t>
+        </is>
+      </c>
       <c r="H4" s="14" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
@@ -2396,13 +2410,7 @@
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
       <c r="D6" s="14" t="n"/>
-      <c r="E6" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Maurice Vannier
-(L103)</t>
-        </is>
-      </c>
+      <c r="E6" s="14" t="n"/>
       <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
@@ -2416,8 +2424,20 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="14" t="n"/>
       <c r="D7" s="14" t="n"/>
-      <c r="E7" s="14" t="n"/>
-      <c r="F7" s="14" t="n"/>
+      <c r="E7" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
+      <c r="F7" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
       <c r="G7" s="14" t="n"/>
       <c r="H7" s="14" t="n"/>
     </row>
@@ -2487,7 +2507,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Room: L101 - Week 2: 13/01/2025 - 19/01/2025</t>
+          <t>Teacher: Vannier_Maurice - Week 2: 13/01/2025 - 19/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -2544,34 +2564,22 @@
           <t>08:15 - 09:45</t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
-      <c r="C3" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
-      <c r="D3" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+      <c r="B3" s="14" t="n"/>
+      <c r="C3" s="14" t="n"/>
+      <c r="D3" s="14" t="n"/>
       <c r="E3" s="14" t="n"/>
-      <c r="F3" s="14" t="n"/>
-      <c r="G3" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Constantin Poussin
-(L101)</t>
+      <c r="F3" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
+      <c r="G3" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
         </is>
       </c>
       <c r="H3" s="14" t="n"/>
@@ -2582,36 +2590,18 @@
           <t>10:00 - 11:30</t>
         </is>
       </c>
-      <c r="B4" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
-      <c r="C4" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+      <c r="B4" s="14" t="n"/>
+      <c r="C4" s="14" t="n"/>
       <c r="D4" s="14" t="n"/>
-      <c r="E4" s="19" t="inlineStr">
+      <c r="E4" s="14" t="n"/>
+      <c r="F4" s="19" t="inlineStr">
         <is>
           <t>Advanced Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
-      <c r="F4" s="14" t="n"/>
-      <c r="G4" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
+      <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
@@ -2634,26 +2624,14 @@
           <t>13:30 - 15:00</t>
         </is>
       </c>
-      <c r="B6" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
+      <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
-      <c r="D6" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
+      <c r="D6" s="14" t="n"/>
       <c r="E6" s="14" t="n"/>
-      <c r="F6" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
+      <c r="F6" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
 (L101)</t>
         </is>
       </c>
@@ -2666,20 +2644,8 @@
           <t>15:15 - 16:45</t>
         </is>
       </c>
-      <c r="B7" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
-      <c r="C7" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+      <c r="B7" s="14" t="n"/>
+      <c r="C7" s="14" t="n"/>
       <c r="D7" s="14" t="n"/>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n"/>
@@ -2693,13 +2659,7 @@
         </is>
       </c>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
+      <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
       <c r="E8" s="14" t="n"/>
       <c r="F8" s="14" t="n"/>
@@ -2712,13 +2672,7 @@
           <t>18:45 - 20:15</t>
         </is>
       </c>
-      <c r="B9" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
+      <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
       <c r="E9" s="14" t="n"/>
@@ -2764,7 +2718,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Room: L101 - Week 1: 06/01/2025 - 12/01/2025</t>
+          <t>Room: L101 - Week 2: 13/01/2025 - 19/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -2822,23 +2776,23 @@
         </is>
       </c>
       <c r="B3" s="14" t="n"/>
-      <c r="C3" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
-      <c r="D3" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
+      <c r="C3" s="14" t="n"/>
+      <c r="D3" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
 (L101)</t>
         </is>
       </c>
       <c r="E3" s="14" t="n"/>
       <c r="F3" s="14" t="n"/>
-      <c r="G3" s="14" t="n"/>
+      <c r="G3" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L101)</t>
+        </is>
+      </c>
       <c r="H3" s="14" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
@@ -2849,15 +2803,15 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n"/>
-      <c r="D4" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
+      <c r="D4" s="14" t="n"/>
+      <c r="E4" s="14" t="n"/>
+      <c r="F4" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
 (L101)</t>
         </is>
       </c>
-      <c r="E4" s="14" t="n"/>
-      <c r="F4" s="14" t="n"/>
       <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
@@ -2881,26 +2835,20 @@
           <t>13:30 - 15:00</t>
         </is>
       </c>
-      <c r="B6" s="19" t="inlineStr">
+      <c r="B6" s="14" t="n"/>
+      <c r="C6" s="14" t="n"/>
+      <c r="D6" s="14" t="n"/>
+      <c r="E6" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L101)</t>
+        </is>
+      </c>
+      <c r="F6" s="19" t="inlineStr">
         <is>
           <t>Advanced Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
-      <c r="C6" s="14" t="n"/>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
-      <c r="E6" s="14" t="n"/>
-      <c r="F6" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
+Maurice Vannier
 (L101)</t>
         </is>
       </c>
@@ -2913,23 +2861,17 @@
           <t>15:15 - 16:45</t>
         </is>
       </c>
-      <c r="B7" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
+      <c r="B7" s="14" t="n"/>
       <c r="C7" s="14" t="n"/>
       <c r="D7" s="14" t="n"/>
-      <c r="E7" s="14" t="n"/>
-      <c r="F7" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
+      <c r="E7" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
 (L101)</t>
         </is>
       </c>
+      <c r="F7" s="14" t="n"/>
       <c r="G7" s="14" t="n"/>
       <c r="H7" s="14" t="n"/>
     </row>
@@ -2942,10 +2884,10 @@
       <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
-      <c r="E8" s="16" t="inlineStr">
+      <c r="E8" s="13" t="inlineStr">
         <is>
           <t>Basic Physics
-Renaud Cerfbeer
+Constantin Poussin
 (L101)</t>
         </is>
       </c>
@@ -2959,13 +2901,7 @@
           <t>18:45 - 20:15</t>
         </is>
       </c>
-      <c r="B9" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Maurice Vannier
-(L101)</t>
-        </is>
-      </c>
+      <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
       <c r="E9" s="14" t="n"/>
@@ -3011,7 +2947,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Room: L103 - Week 1: 06/01/2025 - 12/01/2025</t>
+          <t>Room: L101 - Week 1: 06/01/2025 - 12/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -3069,23 +3005,17 @@
         </is>
       </c>
       <c r="B3" s="14" t="n"/>
-      <c r="C3" s="14" t="n"/>
+      <c r="C3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L101)</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="n"/>
-      <c r="E3" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L103)</t>
-        </is>
-      </c>
+      <c r="E3" s="14" t="n"/>
       <c r="F3" s="14" t="n"/>
-      <c r="G3" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L103)</t>
-        </is>
-      </c>
+      <c r="G3" s="14" t="n"/>
       <c r="H3" s="14" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
@@ -3097,13 +3027,19 @@
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n"/>
       <c r="D4" s="14" t="n"/>
-      <c r="E4" s="14" t="n"/>
+      <c r="E4" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L101)</t>
+        </is>
+      </c>
       <c r="F4" s="14" t="n"/>
-      <c r="G4" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Timothé Solé
-(L103)</t>
+      <c r="G4" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L101)</t>
         </is>
       </c>
       <c r="H4" s="14" t="n"/>
@@ -3130,8 +3066,20 @@
       </c>
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
-      <c r="D6" s="14" t="n"/>
-      <c r="E6" s="14" t="n"/>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L101)</t>
+        </is>
+      </c>
+      <c r="E6" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L101)</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
@@ -3144,13 +3092,7 @@
       </c>
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="14" t="n"/>
-      <c r="D7" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
+      <c r="D7" s="14" t="n"/>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n"/>
       <c r="G7" s="14" t="n"/>
@@ -3162,13 +3104,7 @@
           <t>17:00 - 18:30</t>
         </is>
       </c>
-      <c r="B8" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Constantin Poussin
-(L103)</t>
-        </is>
-      </c>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
       <c r="E8" s="14" t="n"/>
@@ -3185,13 +3121,7 @@
       <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
-      <c r="E9" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Constantin Poussin
-(L103)</t>
-        </is>
-      </c>
+      <c r="E9" s="14" t="n"/>
       <c r="F9" s="14" t="n"/>
       <c r="G9" s="14" t="n"/>
       <c r="H9" s="14" t="n"/>
@@ -3293,15 +3223,21 @@
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="C3" s="14" t="n"/>
+      <c r="D3" s="15" t="inlineStr">
+        <is>
           <t>Basic Maths
-Henri Barbeau
+Timothé Solé
 (L101)</t>
         </is>
       </c>
-      <c r="C3" s="14" t="n"/>
-      <c r="D3" s="14" t="n"/>
       <c r="E3" s="14" t="n"/>
-      <c r="F3" s="15" t="inlineStr">
+      <c r="F3" s="16" t="inlineStr">
         <is>
           <t>Basic Informatics
 Christiane Brunelle
@@ -3310,36 +3246,36 @@
       </c>
       <c r="G3" s="16" t="inlineStr">
         <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L101)</t>
+        </is>
+      </c>
+      <c r="H3" s="14" t="n"/>
+    </row>
+    <row r="4" ht="60" customHeight="1">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>10:00 - 11:30</t>
+        </is>
+      </c>
+      <c r="B4" s="14" t="n"/>
+      <c r="C4" s="13" t="inlineStr">
+        <is>
           <t>Basic Physics
 Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="D4" s="14" t="n"/>
+      <c r="E4" s="14" t="n"/>
+      <c r="F4" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
 (L101)</t>
         </is>
       </c>
-      <c r="H3" s="14" t="n"/>
-    </row>
-    <row r="4" ht="60" customHeight="1">
-      <c r="A4" s="12" t="inlineStr">
-        <is>
-          <t>10:00 - 11:30</t>
-        </is>
-      </c>
-      <c r="B4" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
-      <c r="C4" s="14" t="n"/>
-      <c r="D4" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L102)</t>
-        </is>
-      </c>
-      <c r="E4" s="14" t="n"/>
-      <c r="F4" s="14" t="n"/>
       <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
@@ -3363,29 +3299,35 @@
           <t>13:30 - 15:00</t>
         </is>
       </c>
-      <c r="B6" s="16" t="inlineStr">
+      <c r="B6" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="C6" s="14" t="n"/>
+      <c r="D6" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="E6" s="13" t="inlineStr">
         <is>
           <t>Basic Physics
-Renaud Cerfbeer
+Constantin Poussin
 (L101)</t>
         </is>
       </c>
-      <c r="C6" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L103)</t>
-        </is>
-      </c>
-      <c r="D6" s="14" t="n"/>
-      <c r="E6" s="15" t="inlineStr">
+      <c r="F6" s="16" t="inlineStr">
         <is>
           <t>Basic Informatics
 Christiane Brunelle
 (L102)</t>
         </is>
       </c>
-      <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
     </row>
@@ -3395,22 +3337,22 @@
           <t>15:15 - 16:45</t>
         </is>
       </c>
-      <c r="B7" s="13" t="inlineStr">
+      <c r="B7" s="15" t="inlineStr">
         <is>
           <t>Basic Maths
-Henri Barbeau
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="C7" s="14" t="n"/>
+      <c r="D7" s="14" t="n"/>
+      <c r="E7" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
 (L101)</t>
         </is>
       </c>
-      <c r="C7" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
-      <c r="D7" s="14" t="n"/>
-      <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n"/>
       <c r="G7" s="14" t="n"/>
       <c r="H7" s="14" t="n"/>
@@ -3421,22 +3363,16 @@
           <t>17:00 - 18:30</t>
         </is>
       </c>
-      <c r="B8" s="16" t="inlineStr">
+      <c r="B8" s="14" t="n"/>
+      <c r="C8" s="14" t="n"/>
+      <c r="D8" s="14" t="n"/>
+      <c r="E8" s="13" t="inlineStr">
         <is>
           <t>Basic Physics
-Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
-      <c r="C8" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
+Constantin Poussin
 (L101)</t>
         </is>
       </c>
-      <c r="D8" s="14" t="n"/>
-      <c r="E8" s="14" t="n"/>
       <c r="F8" s="14" t="n"/>
       <c r="G8" s="14" t="n"/>
       <c r="H8" s="14" t="n"/>
@@ -3447,13 +3383,7 @@
           <t>18:45 - 20:15</t>
         </is>
       </c>
-      <c r="B9" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
+      <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
       <c r="E9" s="14" t="n"/>
@@ -3499,7 +3429,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Room: L103 - Week 2: 13/01/2025 - 19/01/2025</t>
+          <t>Room: L102 - Week 2: 13/01/2025 - 19/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -3556,28 +3486,46 @@
           <t>08:15 - 09:45</t>
         </is>
       </c>
-      <c r="B3" s="14" t="n"/>
-      <c r="C3" s="14" t="n"/>
-      <c r="D3" s="14" t="n"/>
-      <c r="E3" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
-(L103)</t>
-        </is>
-      </c>
-      <c r="F3" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L103)</t>
-        </is>
-      </c>
-      <c r="G3" s="17" t="inlineStr">
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="C3" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
+      <c r="D3" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
+      <c r="E3" s="18" t="inlineStr">
         <is>
           <t>Advanced Physics
 Renaud Cerfbeer
-(L103)</t>
+(L102)</t>
+        </is>
+      </c>
+      <c r="F3" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
+      <c r="G3" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
         </is>
       </c>
       <c r="H3" s="14" t="n"/>
@@ -3588,17 +3536,41 @@
           <t>10:00 - 11:30</t>
         </is>
       </c>
-      <c r="B4" s="14" t="n"/>
-      <c r="C4" s="14" t="n"/>
+      <c r="B4" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
+      <c r="C4" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
       <c r="D4" s="17" t="inlineStr">
         <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
+      <c r="E4" s="18" t="inlineStr">
+        <is>
           <t>Advanced Physics
-Constantin Poussin
-(L103)</t>
-        </is>
-      </c>
-      <c r="E4" s="14" t="n"/>
-      <c r="F4" s="14" t="n"/>
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
+      <c r="F4" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
       <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
@@ -3622,23 +3594,35 @@
           <t>13:30 - 15:00</t>
         </is>
       </c>
-      <c r="B6" s="14" t="n"/>
-      <c r="C6" s="13" t="inlineStr">
+      <c r="B6" s="15" t="inlineStr">
         <is>
           <t>Basic Maths
-Henri Barbeau
-(L103)</t>
-        </is>
-      </c>
-      <c r="D6" s="14" t="n"/>
-      <c r="E6" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Maurice Vannier
-(L103)</t>
-        </is>
-      </c>
-      <c r="F6" s="14" t="n"/>
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="C6" s="14" t="n"/>
+      <c r="D6" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="E6" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
+      <c r="F6" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L102)</t>
+        </is>
+      </c>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
     </row>
@@ -3648,7 +3632,13 @@
           <t>15:15 - 16:45</t>
         </is>
       </c>
-      <c r="B7" s="14" t="n"/>
+      <c r="B7" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
       <c r="C7" s="14" t="n"/>
       <c r="D7" s="14" t="n"/>
       <c r="E7" s="14" t="n"/>
@@ -3662,16 +3652,16 @@
           <t>17:00 - 18:30</t>
         </is>
       </c>
-      <c r="B8" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
-      <c r="E8" s="14" t="n"/>
+      <c r="E8" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="F8" s="14" t="n"/>
       <c r="G8" s="14" t="n"/>
       <c r="H8" s="14" t="n"/>
@@ -3682,16 +3672,16 @@
           <t>18:45 - 20:15</t>
         </is>
       </c>
-      <c r="B9" s="17" t="inlineStr">
+      <c r="B9" s="14" t="n"/>
+      <c r="C9" s="14" t="n"/>
+      <c r="D9" s="14" t="n"/>
+      <c r="E9" s="18" t="inlineStr">
         <is>
           <t>Advanced Physics
 Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
-      <c r="C9" s="14" t="n"/>
-      <c r="D9" s="14" t="n"/>
-      <c r="E9" s="14" t="n"/>
+(L102)</t>
+        </is>
+      </c>
       <c r="F9" s="14" t="n"/>
       <c r="G9" s="14" t="n"/>
       <c r="H9" s="14" t="n"/>
@@ -3791,50 +3781,86 @@
           <t>08:15 - 09:45</t>
         </is>
       </c>
-      <c r="B3" s="18" t="inlineStr">
+      <c r="B3" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
+      <c r="C3" s="17" t="inlineStr">
         <is>
           <t>Advanced Maths
 Henri Barbeau
 (L102)</t>
         </is>
       </c>
-      <c r="C3" s="14" t="n"/>
-      <c r="D3" s="14" t="n"/>
-      <c r="E3" s="14" t="n"/>
-      <c r="F3" s="18" t="inlineStr">
+      <c r="D3" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L102)</t>
+        </is>
+      </c>
+      <c r="E3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="F3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="G3" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
+      <c r="H3" s="14" t="n"/>
+    </row>
+    <row r="4" ht="60" customHeight="1">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>10:00 - 11:30</t>
+        </is>
+      </c>
+      <c r="B4" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="C4" s="17" t="inlineStr">
         <is>
           <t>Advanced Maths
 Henri Barbeau
 (L102)</t>
         </is>
       </c>
-      <c r="G3" s="14" t="n"/>
-      <c r="H3" s="14" t="n"/>
-    </row>
-    <row r="4" ht="60" customHeight="1">
-      <c r="A4" s="12" t="inlineStr">
-        <is>
-          <t>10:00 - 11:30</t>
-        </is>
-      </c>
-      <c r="B4" s="14" t="n"/>
-      <c r="C4" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
+      <c r="D4" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L102)</t>
+        </is>
+      </c>
+      <c r="E4" s="14" t="n"/>
+      <c r="F4" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
 Renaud Cerfbeer
 (L102)</t>
         </is>
       </c>
-      <c r="D4" s="14" t="n"/>
-      <c r="E4" s="14" t="n"/>
-      <c r="F4" s="14" t="n"/>
-      <c r="G4" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L102)</t>
-        </is>
-      </c>
+      <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
@@ -3859,15 +3885,27 @@
       </c>
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
-      <c r="D6" s="14" t="n"/>
+      <c r="D6" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
       <c r="E6" s="15" t="inlineStr">
         <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L102)</t>
-        </is>
-      </c>
-      <c r="F6" s="14" t="n"/>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="F6" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
     </row>
@@ -3879,15 +3917,26 @@
       </c>
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="14" t="n"/>
-      <c r="D7" s="14" t="n"/>
-      <c r="E7" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Constantin Poussin
-(L102)</t>
-        </is>
-      </c>
-      <c r="F7" s="14" t="n"/>
+      <c r="D7" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="E7" s="20" t="inlineStr">
+        <is>
+          <t>Basic Informatics (L102)
+Advanced Informatics (L102)</t>
+        </is>
+      </c>
+      <c r="F7" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
       <c r="G7" s="14" t="n"/>
       <c r="H7" s="14" t="n"/>
     </row>
@@ -3897,32 +3946,20 @@
           <t>17:00 - 18:30</t>
         </is>
       </c>
-      <c r="B8" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L102)</t>
-        </is>
-      </c>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
-      <c r="D8" s="13" t="inlineStr">
+      <c r="D8" s="14" t="n"/>
+      <c r="E8" s="15" t="inlineStr">
         <is>
           <t>Basic Maths
-Henri Barbeau
-(L102)</t>
-        </is>
-      </c>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="F8" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
 Constantin Poussin
-(L102)</t>
-        </is>
-      </c>
-      <c r="F8" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Maurice Vannier
 (L102)</t>
         </is>
       </c>
@@ -3938,7 +3975,13 @@
       <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
-      <c r="E9" s="14" t="n"/>
+      <c r="E9" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="F9" s="14" t="n"/>
       <c r="G9" s="14" t="n"/>
       <c r="H9" s="14" t="n"/>
@@ -3981,7 +4024,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Room: L102 - Week 2: 13/01/2025 - 19/01/2025</t>
+          <t>Room: Online - Week 1: 06/01/2025 - 12/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -4054,22 +4097,16 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n"/>
-      <c r="D4" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L102)</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="n"/>
       <c r="E4" s="14" t="n"/>
-      <c r="F4" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
+      <c r="F4" s="14" t="n"/>
+      <c r="G4" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
 Christiane Brunelle
-(L102)</t>
-        </is>
-      </c>
-      <c r="G4" s="14" t="n"/>
+(Online)</t>
+        </is>
+      </c>
       <c r="H4" s="14" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
@@ -4095,13 +4132,200 @@
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
       <c r="D6" s="14" t="n"/>
-      <c r="E6" s="15" t="inlineStr">
+      <c r="E6" s="14" t="n"/>
+      <c r="F6" s="14" t="n"/>
+      <c r="G6" s="14" t="n"/>
+      <c r="H6" s="14" t="n"/>
+    </row>
+    <row r="7" ht="60" customHeight="1">
+      <c r="A7" s="12" t="inlineStr">
+        <is>
+          <t>15:15 - 16:45</t>
+        </is>
+      </c>
+      <c r="B7" s="14" t="n"/>
+      <c r="C7" s="14" t="n"/>
+      <c r="D7" s="14" t="n"/>
+      <c r="E7" s="14" t="n"/>
+      <c r="F7" s="14" t="n"/>
+      <c r="G7" s="14" t="n"/>
+      <c r="H7" s="14" t="n"/>
+    </row>
+    <row r="8" ht="60" customHeight="1">
+      <c r="A8" s="12" t="inlineStr">
+        <is>
+          <t>17:00 - 18:30</t>
+        </is>
+      </c>
+      <c r="B8" s="14" t="n"/>
+      <c r="C8" s="14" t="n"/>
+      <c r="D8" s="14" t="n"/>
+      <c r="E8" s="14" t="n"/>
+      <c r="F8" s="14" t="n"/>
+      <c r="G8" s="14" t="n"/>
+      <c r="H8" s="14" t="n"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="12" t="inlineStr">
+        <is>
+          <t>18:45 - 20:15</t>
+        </is>
+      </c>
+      <c r="B9" s="14" t="n"/>
+      <c r="C9" s="14" t="n"/>
+      <c r="D9" s="14" t="n"/>
+      <c r="E9" s="14" t="n"/>
+      <c r="F9" s="14" t="n"/>
+      <c r="G9" s="14" t="n"/>
+      <c r="H9" s="14" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="H1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="60" customHeight="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>Room: L103 - Week 2: 13/01/2025 - 19/01/2025</t>
+        </is>
+      </c>
+      <c r="H1" s="10" t="inlineStr">
+        <is>
+          <t>Back to Index</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="60" customHeight="1">
+      <c r="A2" s="11" t="inlineStr">
+        <is>
+          <t>Time Slot</t>
+        </is>
+      </c>
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C2" s="11" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E2" s="11" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="F2" s="11" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="G2" s="11" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="H2" s="11" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="60" customHeight="1">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t>08:15 - 09:45</t>
+        </is>
+      </c>
+      <c r="B3" s="14" t="n"/>
+      <c r="C3" s="14" t="n"/>
+      <c r="D3" s="14" t="n"/>
+      <c r="E3" s="14" t="n"/>
+      <c r="F3" s="16" t="inlineStr">
         <is>
           <t>Basic Informatics
 Christiane Brunelle
-(L102)</t>
-        </is>
-      </c>
+(L103)</t>
+        </is>
+      </c>
+      <c r="G3" s="14" t="n"/>
+      <c r="H3" s="14" t="n"/>
+    </row>
+    <row r="4" ht="60" customHeight="1">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>10:00 - 11:30</t>
+        </is>
+      </c>
+      <c r="B4" s="14" t="n"/>
+      <c r="C4" s="14" t="n"/>
+      <c r="D4" s="14" t="n"/>
+      <c r="E4" s="14" t="n"/>
+      <c r="F4" s="14" t="n"/>
+      <c r="G4" s="14" t="n"/>
+      <c r="H4" s="14" t="n"/>
+    </row>
+    <row r="5" ht="60" customHeight="1">
+      <c r="A5" s="12" t="inlineStr">
+        <is>
+          <t>11:45 - 13:15</t>
+        </is>
+      </c>
+      <c r="B5" s="14" t="n"/>
+      <c r="C5" s="14" t="n"/>
+      <c r="D5" s="14" t="n"/>
+      <c r="E5" s="14" t="n"/>
+      <c r="F5" s="14" t="n"/>
+      <c r="G5" s="14" t="n"/>
+      <c r="H5" s="14" t="n"/>
+    </row>
+    <row r="6" ht="60" customHeight="1">
+      <c r="A6" s="12" t="inlineStr">
+        <is>
+          <t>13:30 - 15:00</t>
+        </is>
+      </c>
+      <c r="B6" s="14" t="n"/>
+      <c r="C6" s="14" t="n"/>
+      <c r="D6" s="14" t="n"/>
+      <c r="E6" s="14" t="n"/>
       <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
@@ -4244,29 +4468,35 @@
         </is>
       </c>
       <c r="B3" s="14" t="n"/>
-      <c r="C3" s="14" t="n"/>
+      <c r="C3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L101)</t>
+        </is>
+      </c>
       <c r="D3" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
-      <c r="E3" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L103)</t>
-        </is>
-      </c>
-      <c r="F3" s="14" t="n"/>
-      <c r="G3" s="15" t="inlineStr">
         <is>
           <t>Basic Informatics
 Christiane Brunelle
-(L103)</t>
-        </is>
-      </c>
+(L102)</t>
+        </is>
+      </c>
+      <c r="E3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="F3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="G3" s="14" t="n"/>
       <c r="H3" s="14" t="n"/>
     </row>
     <row r="4" ht="60" customHeight="1">
@@ -4275,28 +4505,28 @@
           <t>10:00 - 11:30</t>
         </is>
       </c>
-      <c r="B4" s="14" t="n"/>
-      <c r="C4" s="16" t="inlineStr">
+      <c r="B4" s="13" t="inlineStr">
         <is>
           <t>Basic Physics
-Renaud Cerfbeer
-(L102)</t>
-        </is>
-      </c>
-      <c r="D4" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L101)</t>
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="C4" s="14" t="n"/>
+      <c r="D4" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(L102)</t>
         </is>
       </c>
       <c r="E4" s="14" t="n"/>
       <c r="F4" s="14" t="n"/>
-      <c r="G4" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Timothé Solé
-(L103)</t>
+      <c r="G4" s="16" t="inlineStr">
+        <is>
+          <t>Basic Informatics
+Christiane Brunelle
+(Online)</t>
         </is>
       </c>
       <c r="H4" s="14" t="n"/>
@@ -4323,40 +4553,46 @@
       </c>
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
-      <c r="D6" s="14" t="n"/>
+      <c r="D6" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
       <c r="E6" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="F6" s="14" t="n"/>
+      <c r="G6" s="14" t="n"/>
+      <c r="H6" s="14" t="n"/>
+    </row>
+    <row r="7" ht="60" customHeight="1">
+      <c r="A7" s="12" t="inlineStr">
+        <is>
+          <t>15:15 - 16:45</t>
+        </is>
+      </c>
+      <c r="B7" s="14" t="n"/>
+      <c r="C7" s="14" t="n"/>
+      <c r="D7" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="E7" s="16" t="inlineStr">
         <is>
           <t>Basic Informatics
 Christiane Brunelle
 (L102)</t>
         </is>
       </c>
-      <c r="F6" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
-      <c r="G6" s="14" t="n"/>
-      <c r="H6" s="14" t="n"/>
-    </row>
-    <row r="7" ht="60" customHeight="1">
-      <c r="A7" s="12" t="inlineStr">
-        <is>
-          <t>15:15 - 16:45</t>
-        </is>
-      </c>
-      <c r="B7" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
-      <c r="C7" s="14" t="n"/>
-      <c r="D7" s="14" t="n"/>
-      <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n"/>
       <c r="G7" s="14" t="n"/>
       <c r="H7" s="14" t="n"/>
@@ -4367,32 +4603,20 @@
           <t>17:00 - 18:30</t>
         </is>
       </c>
-      <c r="B8" s="16" t="inlineStr">
+      <c r="B8" s="14" t="n"/>
+      <c r="C8" s="14" t="n"/>
+      <c r="D8" s="14" t="n"/>
+      <c r="E8" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="F8" s="13" t="inlineStr">
         <is>
           <t>Basic Physics
 Constantin Poussin
-(L103)</t>
-        </is>
-      </c>
-      <c r="C8" s="14" t="n"/>
-      <c r="D8" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L102)</t>
-        </is>
-      </c>
-      <c r="E8" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
-      <c r="F8" s="15" t="inlineStr">
-        <is>
-          <t>Basic Informatics
-Maurice Vannier
 (L102)</t>
         </is>
       </c>
@@ -4511,77 +4735,77 @@
       <c r="B3" s="14" t="n"/>
       <c r="C3" s="17" t="inlineStr">
         <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
+      <c r="D3" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
+      <c r="E3" s="18" t="inlineStr">
+        <is>
           <t>Advanced Physics
 Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
-      <c r="D3" s="18" t="inlineStr">
+(L102)</t>
+        </is>
+      </c>
+      <c r="F3" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
+      <c r="G3" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
+      <c r="H3" s="14" t="n"/>
+    </row>
+    <row r="4" ht="60" customHeight="1">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>10:00 - 11:30</t>
+        </is>
+      </c>
+      <c r="B4" s="17" t="inlineStr">
         <is>
           <t>Advanced Maths
 Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
-      <c r="E3" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
-(L103)</t>
-        </is>
-      </c>
-      <c r="F3" s="14" t="n"/>
-      <c r="G3" s="17" t="inlineStr">
+(L102)</t>
+        </is>
+      </c>
+      <c r="C4" s="14" t="n"/>
+      <c r="D4" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
+      <c r="E4" s="18" t="inlineStr">
         <is>
           <t>Advanced Physics
 Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
-      <c r="H3" s="14" t="n"/>
-    </row>
-    <row r="4" ht="60" customHeight="1">
-      <c r="A4" s="12" t="inlineStr">
-        <is>
-          <t>10:00 - 11:30</t>
-        </is>
-      </c>
-      <c r="B4" s="14" t="n"/>
-      <c r="C4" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
-      <c r="D4" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Constantin Poussin
-(L103)</t>
-        </is>
-      </c>
-      <c r="E4" s="19" t="inlineStr">
+(L102)</t>
+        </is>
+      </c>
+      <c r="F4" s="19" t="inlineStr">
         <is>
           <t>Advanced Informatics
-Christiane Brunelle
-(L101)</t>
-        </is>
-      </c>
-      <c r="F4" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
-(L102)</t>
-        </is>
-      </c>
-      <c r="G4" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
+      <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
@@ -4606,24 +4830,18 @@
       </c>
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
-      <c r="D6" s="17" t="inlineStr">
+      <c r="D6" s="14" t="n"/>
+      <c r="E6" s="18" t="inlineStr">
         <is>
           <t>Advanced Physics
 Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
-      <c r="E6" s="19" t="inlineStr">
+(L102)</t>
+        </is>
+      </c>
+      <c r="F6" s="19" t="inlineStr">
         <is>
           <t>Advanced Informatics
 Maurice Vannier
-(L103)</t>
-        </is>
-      </c>
-      <c r="F6" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
 (L101)</t>
         </is>
       </c>
@@ -4653,7 +4871,13 @@
       <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
-      <c r="E8" s="14" t="n"/>
+      <c r="E8" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="F8" s="14" t="n"/>
       <c r="G8" s="14" t="n"/>
       <c r="H8" s="14" t="n"/>
@@ -4664,16 +4888,16 @@
           <t>18:45 - 20:15</t>
         </is>
       </c>
-      <c r="B9" s="17" t="inlineStr">
+      <c r="B9" s="14" t="n"/>
+      <c r="C9" s="14" t="n"/>
+      <c r="D9" s="14" t="n"/>
+      <c r="E9" s="18" t="inlineStr">
         <is>
           <t>Advanced Physics
 Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
-      <c r="C9" s="14" t="n"/>
-      <c r="D9" s="14" t="n"/>
-      <c r="E9" s="14" t="n"/>
+(L102)</t>
+        </is>
+      </c>
       <c r="F9" s="14" t="n"/>
       <c r="G9" s="14" t="n"/>
       <c r="H9" s="14" t="n"/>
@@ -4773,48 +4997,66 @@
           <t>08:15 - 09:45</t>
         </is>
       </c>
-      <c r="B3" s="18" t="inlineStr">
+      <c r="B3" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L102)</t>
+        </is>
+      </c>
+      <c r="C3" s="17" t="inlineStr">
         <is>
           <t>Advanced Maths
 Henri Barbeau
 (L102)</t>
         </is>
       </c>
-      <c r="C3" s="18" t="inlineStr">
+      <c r="D3" s="14" t="n"/>
+      <c r="E3" s="14" t="n"/>
+      <c r="F3" s="14" t="n"/>
+      <c r="G3" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
+      <c r="H3" s="14" t="n"/>
+    </row>
+    <row r="4" ht="60" customHeight="1">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>10:00 - 11:30</t>
+        </is>
+      </c>
+      <c r="B4" s="14" t="n"/>
+      <c r="C4" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
+(L102)</t>
+        </is>
+      </c>
+      <c r="D4" s="14" t="n"/>
+      <c r="E4" s="17" t="inlineStr">
         <is>
           <t>Advanced Maths
 Henri Barbeau
 (L101)</t>
         </is>
       </c>
-      <c r="D3" s="14" t="n"/>
-      <c r="E3" s="14" t="n"/>
-      <c r="F3" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L102)</t>
-        </is>
-      </c>
-      <c r="G3" s="14" t="n"/>
-      <c r="H3" s="14" t="n"/>
-    </row>
-    <row r="4" ht="60" customHeight="1">
-      <c r="A4" s="12" t="inlineStr">
-        <is>
-          <t>10:00 - 11:30</t>
-        </is>
-      </c>
-      <c r="B4" s="14" t="n"/>
-      <c r="C4" s="14" t="n"/>
-      <c r="D4" s="14" t="n"/>
-      <c r="E4" s="14" t="n"/>
-      <c r="F4" s="14" t="n"/>
-      <c r="G4" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L102)</t>
+      <c r="F4" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
+      <c r="G4" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
+(L101)</t>
         </is>
       </c>
       <c r="H4" s="14" t="n"/>
@@ -4839,23 +5081,29 @@
           <t>13:30 - 15:00</t>
         </is>
       </c>
-      <c r="B6" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
+      <c r="B6" s="14" t="n"/>
+      <c r="C6" s="14" t="n"/>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
 (L101)</t>
         </is>
       </c>
-      <c r="C6" s="14" t="n"/>
-      <c r="D6" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Christiane Brunelle
+      <c r="E6" s="17" t="inlineStr">
+        <is>
+          <t>Advanced Maths
+Henri Barbeau
 (L101)</t>
         </is>
       </c>
-      <c r="E6" s="14" t="n"/>
-      <c r="F6" s="14" t="n"/>
+      <c r="F6" s="18" t="inlineStr">
+        <is>
+          <t>Advanced Physics
+Renaud Cerfbeer
+(L102)</t>
+        </is>
+      </c>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
     </row>
@@ -4867,25 +5115,19 @@
       </c>
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="14" t="n"/>
-      <c r="D7" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
-      <c r="E7" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Constantin Poussin
+      <c r="D7" s="14" t="n"/>
+      <c r="E7" s="19" t="inlineStr">
+        <is>
+          <t>Advanced Informatics
+Maurice Vannier
 (L102)</t>
         </is>
       </c>
       <c r="F7" s="19" t="inlineStr">
         <is>
           <t>Advanced Informatics
-Christiane Brunelle
-(L101)</t>
+Maurice Vannier
+(L102)</t>
         </is>
       </c>
       <c r="G7" s="14" t="n"/>
@@ -4897,22 +5139,10 @@
           <t>17:00 - 18:30</t>
         </is>
       </c>
-      <c r="B8" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L102)</t>
-        </is>
-      </c>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Constantin Poussin
-(L102)</t>
-        </is>
-      </c>
+      <c r="E8" s="14" t="n"/>
       <c r="F8" s="14" t="n"/>
       <c r="G8" s="14" t="n"/>
       <c r="H8" s="14" t="n"/>
@@ -4923,20 +5153,14 @@
           <t>18:45 - 20:15</t>
         </is>
       </c>
-      <c r="B9" s="19" t="inlineStr">
-        <is>
-          <t>Advanced Informatics
-Maurice Vannier
-(L101)</t>
-        </is>
-      </c>
+      <c r="B9" s="14" t="n"/>
       <c r="C9" s="14" t="n"/>
       <c r="D9" s="14" t="n"/>
-      <c r="E9" s="17" t="inlineStr">
+      <c r="E9" s="18" t="inlineStr">
         <is>
           <t>Advanced Physics
-Constantin Poussin
-(L103)</t>
+Renaud Cerfbeer
+(L102)</t>
         </is>
       </c>
       <c r="F9" s="14" t="n"/>
@@ -4981,7 +5205,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Barbeau_Henri - Week 2: 13/01/2025 - 19/01/2025</t>
+          <t>Teacher: Solé_Timothé - Week 2: 13/01/2025 - 19/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -5038,18 +5262,12 @@
           <t>08:15 - 09:45</t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
+      <c r="B3" s="14" t="n"/>
+      <c r="C3" s="14" t="n"/>
+      <c r="D3" s="15" t="inlineStr">
         <is>
           <t>Basic Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
-      <c r="C3" s="14" t="n"/>
-      <c r="D3" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
+Timothé Solé
 (L101)</t>
         </is>
       </c>
@@ -5065,23 +5283,11 @@
         </is>
       </c>
       <c r="B4" s="14" t="n"/>
-      <c r="C4" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+      <c r="C4" s="14" t="n"/>
       <c r="D4" s="14" t="n"/>
       <c r="E4" s="14" t="n"/>
       <c r="F4" s="14" t="n"/>
-      <c r="G4" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+      <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
@@ -5104,23 +5310,23 @@
           <t>13:30 - 15:00</t>
         </is>
       </c>
-      <c r="B6" s="14" t="n"/>
-      <c r="C6" s="13" t="inlineStr">
+      <c r="B6" s="15" t="inlineStr">
         <is>
           <t>Basic Maths
-Henri Barbeau
-(L103)</t>
-        </is>
-      </c>
-      <c r="D6" s="14" t="n"/>
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="C6" s="14" t="n"/>
+      <c r="D6" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
       <c r="E6" s="14" t="n"/>
-      <c r="F6" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+      <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
     </row>
@@ -5130,20 +5336,14 @@
           <t>15:15 - 16:45</t>
         </is>
       </c>
-      <c r="B7" s="13" t="inlineStr">
+      <c r="B7" s="15" t="inlineStr">
         <is>
           <t>Basic Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
-      <c r="C7" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="C7" s="14" t="n"/>
       <c r="D7" s="14" t="n"/>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n"/>
@@ -5216,7 +5416,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Barbeau_Henri - Week 1: 06/01/2025 - 12/01/2025</t>
+          <t>Teacher: Solé_Timothé - Week 1: 06/01/2025 - 12/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -5273,35 +5473,11 @@
           <t>08:15 - 09:45</t>
         </is>
       </c>
-      <c r="B3" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L102)</t>
-        </is>
-      </c>
-      <c r="C3" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+      <c r="B3" s="14" t="n"/>
+      <c r="C3" s="14" t="n"/>
       <c r="D3" s="14" t="n"/>
-      <c r="E3" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L103)</t>
-        </is>
-      </c>
-      <c r="F3" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L102)</t>
-        </is>
-      </c>
+      <c r="E3" s="14" t="n"/>
+      <c r="F3" s="14" t="n"/>
       <c r="G3" s="14" t="n"/>
       <c r="H3" s="14" t="n"/>
     </row>
@@ -5313,22 +5489,10 @@
       </c>
       <c r="B4" s="14" t="n"/>
       <c r="C4" s="14" t="n"/>
-      <c r="D4" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Henri Barbeau
-(L101)</t>
-        </is>
-      </c>
+      <c r="D4" s="14" t="n"/>
       <c r="E4" s="14" t="n"/>
       <c r="F4" s="14" t="n"/>
-      <c r="G4" s="18" t="inlineStr">
-        <is>
-          <t>Advanced Maths
-Henri Barbeau
-(L102)</t>
-        </is>
-      </c>
+      <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
@@ -5353,8 +5517,20 @@
       </c>
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
-      <c r="D6" s="14" t="n"/>
-      <c r="E6" s="14" t="n"/>
+      <c r="D6" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
+      <c r="E6" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
@@ -5367,7 +5543,13 @@
       </c>
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="14" t="n"/>
-      <c r="D7" s="14" t="n"/>
+      <c r="D7" s="15" t="inlineStr">
+        <is>
+          <t>Basic Maths
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n"/>
       <c r="G7" s="14" t="n"/>
@@ -5381,14 +5563,14 @@
       </c>
       <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
-      <c r="D8" s="13" t="inlineStr">
+      <c r="D8" s="14" t="n"/>
+      <c r="E8" s="15" t="inlineStr">
         <is>
           <t>Basic Maths
-Henri Barbeau
-(L102)</t>
-        </is>
-      </c>
-      <c r="E8" s="14" t="n"/>
+Timothé Solé
+(L102)</t>
+        </is>
+      </c>
       <c r="F8" s="14" t="n"/>
       <c r="G8" s="14" t="n"/>
       <c r="H8" s="14" t="n"/>
@@ -5445,7 +5627,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Solé_Timothé - Week 1: 06/01/2025 - 12/01/2025</t>
+          <t>Teacher: Poussin_Constantin - Week 1: 06/01/2025 - 12/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -5503,10 +5685,28 @@
         </is>
       </c>
       <c r="B3" s="14" t="n"/>
-      <c r="C3" s="14" t="n"/>
+      <c r="C3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L101)</t>
+        </is>
+      </c>
       <c r="D3" s="14" t="n"/>
-      <c r="E3" s="14" t="n"/>
-      <c r="F3" s="14" t="n"/>
+      <c r="E3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
+      <c r="F3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
       <c r="G3" s="14" t="n"/>
       <c r="H3" s="14" t="n"/>
     </row>
@@ -5516,18 +5716,18 @@
           <t>10:00 - 11:30</t>
         </is>
       </c>
-      <c r="B4" s="14" t="n"/>
+      <c r="B4" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
       <c r="C4" s="14" t="n"/>
       <c r="D4" s="14" t="n"/>
       <c r="E4" s="14" t="n"/>
       <c r="F4" s="14" t="n"/>
-      <c r="G4" s="13" t="inlineStr">
-        <is>
-          <t>Basic Maths
-Timothé Solé
-(L103)</t>
-        </is>
-      </c>
+      <c r="G4" s="14" t="n"/>
       <c r="H4" s="14" t="n"/>
     </row>
     <row r="5" ht="60" customHeight="1">
@@ -5582,7 +5782,13 @@
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
       <c r="E8" s="14" t="n"/>
-      <c r="F8" s="14" t="n"/>
+      <c r="F8" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
       <c r="G8" s="14" t="n"/>
       <c r="H8" s="14" t="n"/>
     </row>
@@ -5638,7 +5844,7 @@
     <row r="1" ht="60" customHeight="1">
       <c r="A1" s="9" t="inlineStr">
         <is>
-          <t>Teacher: Cerfbeer_Renaud - Week 1: 06/01/2025 - 12/01/2025</t>
+          <t>Teacher: Poussin_Constantin - Week 2: 13/01/2025 - 19/01/2025</t>
         </is>
       </c>
       <c r="H1" s="10" t="inlineStr">
@@ -5695,15 +5901,15 @@
           <t>08:15 - 09:45</t>
         </is>
       </c>
-      <c r="B3" s="14" t="n"/>
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L102)</t>
+        </is>
+      </c>
       <c r="C3" s="14" t="n"/>
-      <c r="D3" s="16" t="inlineStr">
-        <is>
-          <t>Basic Physics
-Renaud Cerfbeer
-(L101)</t>
-        </is>
-      </c>
+      <c r="D3" s="14" t="n"/>
       <c r="E3" s="14" t="n"/>
       <c r="F3" s="14" t="n"/>
       <c r="G3" s="14" t="n"/>
@@ -5716,10 +5922,10 @@
         </is>
       </c>
       <c r="B4" s="14" t="n"/>
-      <c r="C4" s="16" t="inlineStr">
+      <c r="C4" s="13" t="inlineStr">
         <is>
           <t>Basic Physics
-Renaud Cerfbeer
+Constantin Poussin
 (L102)</t>
         </is>
       </c>
@@ -5752,7 +5958,13 @@
       <c r="B6" s="14" t="n"/>
       <c r="C6" s="14" t="n"/>
       <c r="D6" s="14" t="n"/>
-      <c r="E6" s="14" t="n"/>
+      <c r="E6" s="13" t="inlineStr">
+        <is>
+          <t>Basic Physics
+Constantin Poussin
+(L101)</t>
+        </is>
+      </c>
       <c r="F6" s="14" t="n"/>
       <c r="G6" s="14" t="n"/>
       <c r="H6" s="14" t="n"/>
@@ -5763,22 +5975,16 @@
           <t>15:15 - 16:45</t>
         </is>
       </c>
-      <c r="B7" s="16" t="inlineStr">
+      <c r="B7" s="14" t="n"/>
+      <c r="C7" s="14" t="n"/>
+      <c r="D7" s="14" t="n"/>
+      <c r="E7" s="13" t="inlineStr">
         <is>
           <t>Basic Physics
-Renaud Cerfbeer
+Constantin Poussin
 (L101)</t>
         </is>
       </c>
-      <c r="C7" s="14" t="n"/>
-      <c r="D7" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L103)</t>
-        </is>
-      </c>
-      <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n"/>
       <c r="G7" s="14" t="n"/>
       <c r="H7" s="14" t="n"/>
@@ -5789,19 +5995,13 @@
           <t>17:00 - 18:30</t>
         </is>
       </c>
-      <c r="B8" s="17" t="inlineStr">
-        <is>
-          <t>Advanced Physics
-Renaud Cerfbeer
-(L102)</t>
-        </is>
-      </c>
+      <c r="B8" s="14" t="n"/>
       <c r="C8" s="14" t="n"/>
       <c r="D8" s="14" t="n"/>
-      <c r="E8" s="16" t="inlineStr">
+      <c r="E8" s="13" t="inlineStr">
         <is>
           <t>Basic Physics
-Renaud Cerfbeer
+Constantin Poussin
 (L101)</t>
         </is>
       </c>

</xml_diff>